<commit_message>
Loop Changes Pseudo and Sensible Heat Gain from PV roof
</commit_message>
<xml_diff>
--- a/cea/databases/WB/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/WB/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\WB\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7183724-3CA9-4F2A-9855-633298D2EB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA58AD-2BC2-4185-BA2D-3488BC6C31C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="3540" windowWidth="21600" windowHeight="11835" tabRatio="785" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="785" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="116">
   <si>
     <t>type_hs</t>
   </si>
@@ -379,6 +379,15 @@
   </si>
   <si>
     <t>MULTIRES_LOW_R31_STND_AC</t>
+  </si>
+  <si>
+    <t>00|00</t>
+  </si>
+  <si>
+    <t>01|01</t>
+  </si>
+  <si>
+    <t>31|12</t>
   </si>
 </sst>
 </file>
@@ -1559,11 +1568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2951,8 +2960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1048560"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,16 +3095,16 @@
         <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3118,16 +3127,16 @@
         <v>33</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3150,16 +3159,16 @@
         <v>33</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3182,16 +3191,16 @@
         <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3214,16 +3223,16 @@
         <v>33</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3246,16 +3255,16 @@
         <v>33</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3278,16 +3287,16 @@
         <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3310,16 +3319,16 @@
         <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3438,16 +3447,16 @@
         <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3470,16 +3479,16 @@
         <v>33</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3502,16 +3511,16 @@
         <v>33</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3534,16 +3543,16 @@
         <v>96</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3566,16 +3575,16 @@
         <v>33</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3598,16 +3607,16 @@
         <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3630,16 +3639,16 @@
         <v>33</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finalize DB Thermal Params
</commit_message>
<xml_diff>
--- a/cea/databases/WB/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/WB/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\WB\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA58AD-2BC2-4185-BA2D-3488BC6C31C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE4012-DED7-4CCB-8B9A-1A0E48742BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="785" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="127">
   <si>
     <t>type_hs</t>
   </si>
@@ -339,12 +339,6 @@
     <t>HVAC_VENTILATION_AS5</t>
   </si>
   <si>
-    <t>01|05</t>
-  </si>
-  <si>
-    <t>01|10</t>
-  </si>
-  <si>
     <t>HVAC_HOTWATER_AS2</t>
   </si>
   <si>
@@ -357,21 +351,12 @@
     <t>HVAC_CONTROLLER_AS1</t>
   </si>
   <si>
-    <t>30|04</t>
-  </si>
-  <si>
-    <t>30|09</t>
-  </si>
-  <si>
     <t>SUPPLY_HOTWATER_AS3</t>
   </si>
   <si>
     <t>SUPPLY_HEATING_AS3</t>
   </si>
   <si>
-    <t>SUPPLY_HEATING_AS7</t>
-  </si>
-  <si>
     <t>SUPPLY_COOLING_AS0</t>
   </si>
   <si>
@@ -388,6 +373,54 @@
   </si>
   <si>
     <t>31|12</t>
+  </si>
+  <si>
+    <t>MULTIRES_LOW_R41_STND_AC</t>
+  </si>
+  <si>
+    <t>MULTIRES_HIGH_R41_STND_AC</t>
+  </si>
+  <si>
+    <t>15|06</t>
+  </si>
+  <si>
+    <t>14|06</t>
+  </si>
+  <si>
+    <t>15|09</t>
+  </si>
+  <si>
+    <t>16|09</t>
+  </si>
+  <si>
+    <t>MULTIRES_LOW_R40_STND_AC</t>
+  </si>
+  <si>
+    <t>MULTIRES_HIGH_R40_STND_AC</t>
+  </si>
+  <si>
+    <t>COOLING WILL BECOME STND</t>
+  </si>
+  <si>
+    <t>NET ZERO READY BUILDINGS</t>
+  </si>
+  <si>
+    <t>OFFICE_R41_STND_AC</t>
+  </si>
+  <si>
+    <t>ROOF_AS23</t>
+  </si>
+  <si>
+    <t>WALL_AS20</t>
+  </si>
+  <si>
+    <t>WINDOW_AS4</t>
+  </si>
+  <si>
+    <t>SUPPLY_HEATING_AS11</t>
+  </si>
+  <si>
+    <t>SUPPLY_HOTWATER_AS11</t>
   </si>
 </sst>
 </file>
@@ -1263,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,10 +1566,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C22" s="12">
         <v>2019</v>
@@ -1547,16 +1580,86 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C23" s="12">
         <v>2019</v>
       </c>
       <c r="D23" s="12">
         <v>2020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="12">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="12">
+        <v>2032</v>
+      </c>
+      <c r="D26" s="12">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="12">
+        <v>2032</v>
+      </c>
+      <c r="D27" s="12">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="12">
+        <v>2032</v>
+      </c>
+      <c r="D28" s="12">
+        <v>2099</v>
       </c>
     </row>
   </sheetData>
@@ -1566,13 +1669,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,7 +2936,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>64</v>
@@ -2892,7 +2995,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>63</v>
@@ -2946,6 +3049,301 @@
         <v>0.4</v>
       </c>
       <c r="S23" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="R27" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S27" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S28" s="2">
         <v>0.4</v>
       </c>
     </row>
@@ -2960,8 +3358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1048560"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,25 +3420,25 @@
         <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3051,28 +3449,28 @@
         <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3083,28 +3481,28 @@
         <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3115,28 +3513,28 @@
         <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3147,28 +3545,28 @@
         <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3179,10 +3577,10 @@
         <v>97</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>35</v>
@@ -3191,16 +3589,16 @@
         <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3211,28 +3609,28 @@
         <v>97</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3243,28 +3641,28 @@
         <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3275,10 +3673,10 @@
         <v>97</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>35</v>
@@ -3287,16 +3685,16 @@
         <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3307,10 +3705,10 @@
         <v>97</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>35</v>
@@ -3319,16 +3717,16 @@
         <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3342,25 +3740,25 @@
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3374,25 +3772,25 @@
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3406,25 +3804,25 @@
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3435,28 +3833,28 @@
         <v>94</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3467,28 +3865,28 @@
         <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3499,28 +3897,28 @@
         <v>97</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3531,10 +3929,10 @@
         <v>97</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>95</v>
@@ -3543,16 +3941,16 @@
         <v>96</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3563,28 +3961,28 @@
         <v>97</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3595,28 +3993,28 @@
         <v>97</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3627,10 +4025,10 @@
         <v>97</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>35</v>
@@ -3639,21 +4037,21 @@
         <v>33</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>97</v>
@@ -3662,30 +4060,30 @@
         <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>97</v>
@@ -3694,25 +4092,185 @@
         <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>106</v>
+      <c r="E24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="1048560" spans="5:5" x14ac:dyDescent="0.25">
@@ -3730,7 +4288,7 @@
   <dimension ref="A1:E1048559"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3764,10 +4322,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>30</v>
@@ -3781,10 +4339,10 @@
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
@@ -3798,13 +4356,13 @@
         <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>29</v>
@@ -3815,13 +4373,13 @@
         <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>29</v>
@@ -3832,13 +4390,13 @@
         <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>29</v>
@@ -3849,13 +4407,13 @@
         <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
@@ -3866,13 +4424,13 @@
         <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
@@ -3883,13 +4441,13 @@
         <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>29</v>
@@ -3900,13 +4458,13 @@
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>29</v>
@@ -3917,13 +4475,13 @@
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>29</v>
@@ -3934,10 +4492,10 @@
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
@@ -3951,10 +4509,10 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>30</v>
@@ -3968,10 +4526,10 @@
         <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>30</v>
@@ -3985,13 +4543,13 @@
         <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>29</v>
@@ -4002,13 +4560,13 @@
         <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>29</v>
@@ -4019,13 +4577,13 @@
         <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>29</v>
@@ -4036,13 +4594,13 @@
         <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>29</v>
@@ -4053,13 +4611,13 @@
         <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>29</v>
@@ -4070,13 +4628,13 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>29</v>
@@ -4087,13 +4645,13 @@
         <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>29</v>
@@ -4101,13 +4659,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>30</v>
@@ -4118,18 +4676,103 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>